<commit_message>
present check fix + extra translations
</commit_message>
<xml_diff>
--- a/Package/LangMod/EN/SourcePadoru.xlsx
+++ b/Package/LangMod/EN/SourcePadoru.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Chara" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="CharaText" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Thing" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Race" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="General" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Chara!$B$3:$AG$3</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="196">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -635,6 +636,24 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text_JP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">padoru_greet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umu~! You get a present too, Merry~!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">padoru_bye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you!</t>
   </si>
 </sst>
 </file>
@@ -2748,7 +2767,7 @@
   </sheetPr>
   <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -3213,4 +3232,81 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="13.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>